<commit_message>
Se han hecho nuevas modificaciones
</commit_message>
<xml_diff>
--- a/Alumnos.xlsx
+++ b/Alumnos.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PNFHNuevo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PNFH\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D04EE-0F91-4168-9767-3A089974130F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,46 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>estatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saul </t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>Howland</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>Patch</t>
-  </si>
-  <si>
-    <t>Cipriano</t>
-  </si>
-  <si>
-    <t>Aegan</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Ares</t>
-  </si>
-  <si>
-    <t>Hidago</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>Traynor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>cedula_alumno</t>
   </si>
@@ -75,17 +36,119 @@
     <t>apellido_alumno</t>
   </si>
   <si>
-    <t>telefono_alumno</t>
-  </si>
-  <si>
     <t>trayecto_alumno</t>
+  </si>
+  <si>
+    <t>25421667</t>
+  </si>
+  <si>
+    <t>HAISBEL YOELIMAR</t>
+  </si>
+  <si>
+    <t>ABAD GUEDEZ</t>
+  </si>
+  <si>
+    <t>28021462</t>
+  </si>
+  <si>
+    <t>YENIFER FRAGNIMAR</t>
+  </si>
+  <si>
+    <t>ADAN VARGAS</t>
+  </si>
+  <si>
+    <t>26898084</t>
+  </si>
+  <si>
+    <t>ALEXANDER MANUEL</t>
+  </si>
+  <si>
+    <t>AGUILAR COLMENARES</t>
+  </si>
+  <si>
+    <t>29895603</t>
+  </si>
+  <si>
+    <t>OSYARLY DEL VALLE</t>
+  </si>
+  <si>
+    <t>TORREALBA SANTIAGO</t>
+  </si>
+  <si>
+    <t>27586008</t>
+  </si>
+  <si>
+    <t>WILMER JOSE</t>
+  </si>
+  <si>
+    <t>VALENZUELA FREITEZ</t>
+  </si>
+  <si>
+    <t>27217754</t>
+  </si>
+  <si>
+    <t>DARIANNYS JOSEFINA</t>
+  </si>
+  <si>
+    <t>VARGAS MARTINEZ</t>
+  </si>
+  <si>
+    <t>26370490</t>
+  </si>
+  <si>
+    <t>PAOLA CAROLINA</t>
+  </si>
+  <si>
+    <t>AGUERO COLMENAREZ</t>
+  </si>
+  <si>
+    <t>BARBARA SOMEIDY</t>
+  </si>
+  <si>
+    <t>ALVARADO CHAVEZ</t>
+  </si>
+  <si>
+    <t>28256888</t>
+  </si>
+  <si>
+    <t>HERITMAR YOESLYN</t>
+  </si>
+  <si>
+    <t>ALVARADO NAVAS</t>
+  </si>
+  <si>
+    <t>25630466</t>
+  </si>
+  <si>
+    <t>REIMARY JOSNELY</t>
+  </si>
+  <si>
+    <t>BARCOS RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>17380052</t>
+  </si>
+  <si>
+    <t>ANDY YIXON</t>
+  </si>
+  <si>
+    <t>DORTA SAAVEDRA</t>
+  </si>
+  <si>
+    <t>27411146</t>
+  </si>
+  <si>
+    <t>MICHELE ANTONIO</t>
+  </si>
+  <si>
+    <t>FIORE PEÑA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +163,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,9 +190,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,175 +482,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="4" max="5" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>789068</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>456</v>
-      </c>
-      <c r="E2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>154328</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>20045024</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>365754</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>567542</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>12345</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>765282</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>7654323</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>862547</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>764234</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5432287</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>8765423</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>